<commit_message>
Minor update: cleaned few comments
</commit_message>
<xml_diff>
--- a/testdata/testdata.xlsx
+++ b/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Test_Flight_Script\Playwright\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F408D3D-8EB6-4C0A-ADBA-D29E86DC63F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C941CD7B-EC79-4CF7-808C-F9E62E378308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30380" yWindow="-7020" windowWidth="29310" windowHeight="16200" xr2:uid="{4966BF41-F4AF-473E-A82F-A15B8A0236D2}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="19848" windowHeight="11292" xr2:uid="{4966BF41-F4AF-473E-A82F-A15B8A0236D2}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -58,10 +58,10 @@
     <t>CICD</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Firefox</t>
   </si>
 </sst>
 </file>
@@ -925,7 +925,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,10 +979,10 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>